<commit_message>
Prices(Keytool) begun/ Animations Product
</commit_message>
<xml_diff>
--- a/PureProductCalculation.xlsx
+++ b/PureProductCalculation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fa2acab9f6e02fa/Dokumente/Schule/2022-23/Junior Companie/Pure/Metal Wallet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fa2acab9f6e02fa/Dokumente/Schule/2022-23/Junior Companie/Pure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8B38597E-3AD7-4822-ADE9-8DC3B9CAEE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A3300C1-08FD-4168-A9C0-76890B917B3E}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{8B38597E-3AD7-4822-ADE9-8DC3B9CAEE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040565E4-A3B2-45E1-A092-ED0C8AFEAB48}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C5F72F3D-9789-4E2A-BA39-C605A7F3DDDC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Comment</t>
   </si>
@@ -141,13 +141,49 @@
   </si>
   <si>
     <t>Gewinn(-USt):</t>
+  </si>
+  <si>
+    <t>Front_Plate</t>
+  </si>
+  <si>
+    <t>Back_Plate</t>
+  </si>
+  <si>
+    <t>Spacer_Big</t>
+  </si>
+  <si>
+    <t>Spacer_Small</t>
+  </si>
+  <si>
+    <t>Chainhole</t>
+  </si>
+  <si>
+    <t>Hülsenmutter</t>
+  </si>
+  <si>
+    <t>Schraube</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>Selling Price:</t>
+  </si>
+  <si>
+    <t>Gewinn</t>
+  </si>
+  <si>
+    <t>Produktions kosten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +199,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +262,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -249,11 +322,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -277,10 +351,21 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -595,7 +680,7 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,12 +1656,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0D6BF1-7B05-48A8-8F90-94992644C689}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="8" width="11.5546875" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="19">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="G2" s="19">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H2" s="19">
+        <v>103.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="G3" s="19">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H3" s="19">
+        <v>103.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="19">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="19">
+        <v>13.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="25" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="19">
+        <f>SUM(E2:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="19">
+        <f>SUM(F2:F21)</f>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G26" s="19">
+        <f>SUM(G2:G21)</f>
+        <v>64.06</v>
+      </c>
+      <c r="H26" s="19">
+        <f>SUM(H2:H21)</f>
+        <v>207.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+    </row>
+    <row r="31" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="23">
+        <f>$B$28-E26</f>
+        <v>20</v>
+      </c>
+      <c r="F31" s="23">
+        <f>$B$28*50-F26</f>
+        <v>981.1</v>
+      </c>
+      <c r="G31" s="23">
+        <f>$B$28*100-G26</f>
+        <v>1935.94</v>
+      </c>
+      <c r="H31" s="23">
+        <f>$B$28*500-H26</f>
+        <v>9792.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>